<commit_message>
add scenario analyses, update results
</commit_message>
<xml_diff>
--- a/dmsan/bwaise/results/MCDA_baseline.xlsx
+++ b/dmsan/bwaise/results/MCDA_baseline.xlsx
@@ -752,13 +752,13 @@
         <v>55</v>
       </c>
       <c r="D4">
-        <v>0.5789427410046413</v>
+        <v>0.4431831111395371</v>
       </c>
       <c r="E4">
-        <v>0.7027404356704336</v>
+        <v>0.6209707718945657</v>
       </c>
       <c r="F4">
-        <v>0.3456893535593643</v>
+        <v>0.4216145211398413</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -772,7 +772,7 @@
         <v>56</v>
       </c>
       <c r="D5">
-        <v>0.7727396798433098</v>
+        <v>0.7523279998200449</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -792,7 +792,7 @@
         <v>57</v>
       </c>
       <c r="D6">
-        <v>0.3834921812874742</v>
+        <v>0.383492181287474</v>
       </c>
       <c r="E6">
         <v>0.9807105925721955</v>
@@ -812,13 +812,13 @@
         <v>58</v>
       </c>
       <c r="D7">
-        <v>0.6649289277222019</v>
+        <v>0.6499145417213249</v>
       </c>
       <c r="E7">
-        <v>0.8836742013540934</v>
+        <v>0.8778272545851326</v>
       </c>
       <c r="F7">
-        <v>0.1268798121051887</v>
+        <v>0.1323819684936061</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -852,13 +852,13 @@
         <v>60</v>
       </c>
       <c r="D9">
-        <v>0.4313003555088307</v>
+        <v>0.3620185166548159</v>
       </c>
       <c r="E9">
-        <v>0.6504473513943876</v>
+        <v>0.6154564462793018</v>
       </c>
       <c r="F9">
-        <v>0.3769486482355294</v>
+        <v>0.4122532093345651</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -872,13 +872,13 @@
         <v>61</v>
       </c>
       <c r="D10">
-        <v>0.7116269806598531</v>
+        <v>0.6921888206727864</v>
       </c>
       <c r="E10">
-        <v>0.8797070830114139</v>
+        <v>0.8737372697874098</v>
       </c>
       <c r="F10">
-        <v>0.1311815594805819</v>
+        <v>0.136786239334902</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -892,13 +892,13 @@
         <v>62</v>
       </c>
       <c r="D11">
-        <v>0.562703930687056</v>
+        <v>0.4721356533617872</v>
       </c>
       <c r="E11">
-        <v>0.644220785002087</v>
+        <v>0.5857689352793057</v>
       </c>
       <c r="F11">
-        <v>0.3842596229456239</v>
+        <v>0.441314105938786</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -912,13 +912,13 @@
         <v>63</v>
       </c>
       <c r="D12">
-        <v>0.7638397502828135</v>
+        <v>0.7447688187902374</v>
       </c>
       <c r="E12">
-        <v>0.9250954099776187</v>
+        <v>0.9259958224920952</v>
       </c>
       <c r="F12">
-        <v>0.07490459002238133</v>
+        <v>0.07400417750790486</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -932,13 +932,13 @@
         <v>64</v>
       </c>
       <c r="D13">
-        <v>0.4046322827814373</v>
+        <v>0.4046322827814371</v>
       </c>
       <c r="E13">
-        <v>0.7896374176788841</v>
+        <v>0.789637417678884</v>
       </c>
       <c r="F13">
-        <v>0.210362582321116</v>
+        <v>0.2103625823211161</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -952,13 +952,13 @@
         <v>65</v>
       </c>
       <c r="D14">
-        <v>0.4313003555088307</v>
+        <v>0.3620185166548159</v>
       </c>
       <c r="E14">
-        <v>0.6504473513943876</v>
+        <v>0.6154564462793018</v>
       </c>
       <c r="F14">
-        <v>0.3769486482355294</v>
+        <v>0.4122532093345651</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -972,13 +972,13 @@
         <v>61</v>
       </c>
       <c r="D15">
-        <v>0.7116269806598531</v>
+        <v>0.6921888206727864</v>
       </c>
       <c r="E15">
-        <v>0.8797070830114139</v>
+        <v>0.8737372697874098</v>
       </c>
       <c r="F15">
-        <v>0.1311815594805819</v>
+        <v>0.136786239334902</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -992,13 +992,13 @@
         <v>66</v>
       </c>
       <c r="D16">
-        <v>0.6897898574702276</v>
+        <v>0.6729456182270112</v>
       </c>
       <c r="E16">
-        <v>0.9032542014993279</v>
+        <v>0.8954214936130447</v>
       </c>
       <c r="F16">
-        <v>0.1075312231759819</v>
+        <v>0.1147919572510599</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1012,13 +1012,13 @@
         <v>67</v>
       </c>
       <c r="D17">
-        <v>0.4492239821279781</v>
+        <v>0.4126776354512215</v>
       </c>
       <c r="E17">
-        <v>0.759245312062826</v>
+        <v>0.7329567446632728</v>
       </c>
       <c r="F17">
-        <v>0.2631697695064517</v>
+        <v>0.2883098614051222</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1032,13 +1032,13 @@
         <v>68</v>
       </c>
       <c r="D18">
-        <v>0.6678537339646711</v>
+        <v>0.652467036162367</v>
       </c>
       <c r="E18">
-        <v>0.9024398810260374</v>
+        <v>0.8948223230462478</v>
       </c>
       <c r="F18">
-        <v>0.1106678395041611</v>
+        <v>0.1175278946680752</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1052,13 +1052,13 @@
         <v>69</v>
       </c>
       <c r="D19">
-        <v>0.6936568252932345</v>
+        <v>0.6763014222131597</v>
       </c>
       <c r="E19">
-        <v>0.9300399298690788</v>
+        <v>0.9182816825663566</v>
       </c>
       <c r="F19">
-        <v>0.08540912935330684</v>
+        <v>0.09536521761552316</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1072,13 +1072,13 @@
         <v>70</v>
       </c>
       <c r="D20">
-        <v>0.7001039617756547</v>
+        <v>0.6872596566604285</v>
       </c>
       <c r="E20">
-        <v>0.9944827240598939</v>
+        <v>0.9945488454708578</v>
       </c>
       <c r="F20">
-        <v>0.005517275940106141</v>
+        <v>0.005451154529142241</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1092,13 +1092,13 @@
         <v>71</v>
       </c>
       <c r="D21">
-        <v>0.3957415396897831</v>
+        <v>0.357159580321769</v>
       </c>
       <c r="E21">
-        <v>0.7689014408727128</v>
+        <v>0.7450870790206342</v>
       </c>
       <c r="F21">
-        <v>0.2586278537501466</v>
+        <v>0.2811931101015958</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1112,13 +1112,13 @@
         <v>72</v>
       </c>
       <c r="D22">
-        <v>0.4110134828132983</v>
+        <v>0.3141296112295865</v>
       </c>
       <c r="E22">
-        <v>0.6830056352698829</v>
+        <v>0.6405381660692044</v>
       </c>
       <c r="F22">
-        <v>0.3532591481256503</v>
+        <v>0.3952126938577485</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1132,13 +1132,13 @@
         <v>73</v>
       </c>
       <c r="D23">
-        <v>0.4402878673178685</v>
+        <v>0.3977658100762115</v>
       </c>
       <c r="E23">
-        <v>0.8140994602824556</v>
+        <v>0.7779344526405685</v>
       </c>
       <c r="F23">
-        <v>0.2211069320867239</v>
+        <v>0.2529864858380443</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1152,13 +1152,13 @@
         <v>74</v>
       </c>
       <c r="D24">
-        <v>0.7580585000559376</v>
+        <v>0.7328119078577248</v>
       </c>
       <c r="E24">
-        <v>0.9275634087782187</v>
+        <v>0.9154102190182059</v>
       </c>
       <c r="F24">
-        <v>0.08845651445677997</v>
+        <v>0.09871345336491412</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1172,13 +1172,13 @@
         <v>75</v>
       </c>
       <c r="D25">
-        <v>0.6722914776694424</v>
+        <v>0.6611790462448828</v>
       </c>
       <c r="E25">
-        <v>0.9259987941352953</v>
+        <v>0.9268056466598925</v>
       </c>
       <c r="F25">
-        <v>0.07821070495604923</v>
+        <v>0.07735996034522688</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1192,13 +1192,13 @@
         <v>76</v>
       </c>
       <c r="D26">
-        <v>0.7256991021961471</v>
+        <v>0.7103339116391424</v>
       </c>
       <c r="E26">
-        <v>0.923348588345312</v>
+        <v>0.9242508536484528</v>
       </c>
       <c r="F26">
-        <v>0.08102485277281603</v>
+        <v>0.08007335687116421</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1212,13 +1212,13 @@
         <v>77</v>
       </c>
       <c r="D27">
-        <v>0.7166858328010987</v>
+        <v>0.6965069871685858</v>
       </c>
       <c r="E27">
-        <v>0.8990544048547874</v>
+        <v>0.8912367314413862</v>
       </c>
       <c r="F27">
-        <v>0.1144913900547553</v>
+        <v>0.1215120652142653</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1252,13 +1252,13 @@
         <v>79</v>
       </c>
       <c r="D29">
-        <v>0.5448708593564857</v>
+        <v>0.4992126290541916</v>
       </c>
       <c r="E29">
-        <v>0.5821877653052189</v>
+        <v>0.5487710217178979</v>
       </c>
       <c r="F29">
-        <v>0.4307089465655795</v>
+        <v>0.4642226902831631</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1272,13 +1272,13 @@
         <v>80</v>
       </c>
       <c r="D30">
-        <v>0.7414716407350769</v>
+        <v>0.7254007048602344</v>
       </c>
       <c r="E30">
-        <v>0.861874234278724</v>
+        <v>0.8633910668752239</v>
       </c>
       <c r="F30">
-        <v>0.1381257657212759</v>
+        <v>0.136608933124776</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1292,13 +1292,13 @@
         <v>81</v>
       </c>
       <c r="D31">
-        <v>0.4411585591738891</v>
+        <v>0.441158559173889</v>
       </c>
       <c r="E31">
-        <v>0.67559717209394</v>
+        <v>0.6755971720939401</v>
       </c>
       <c r="F31">
-        <v>0.3244028279060598</v>
+        <v>0.32440282790606</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1315,7 +1315,7 @@
         <v>0.2052027779755892</v>
       </c>
       <c r="E32">
-        <v>0.6443363925673762</v>
+        <v>0.6443363925673763</v>
       </c>
       <c r="F32">
         <v>0.3772071169015823</v>
@@ -1332,13 +1332,13 @@
         <v>83</v>
       </c>
       <c r="D33">
-        <v>0.2855894521678429</v>
+        <v>0.2184711574160119</v>
       </c>
       <c r="E33">
-        <v>0.6700678473168051</v>
+        <v>0.6526356209817371</v>
       </c>
       <c r="F33">
-        <v>0.3589464005789227</v>
+        <v>0.3769164705897979</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1352,13 +1352,13 @@
         <v>84</v>
       </c>
       <c r="D34">
-        <v>0.6418101286520884</v>
+        <v>0.6318552249037735</v>
       </c>
       <c r="E34">
-        <v>0.8621648075780428</v>
+        <v>0.8635723314934812</v>
       </c>
       <c r="F34">
-        <v>0.1455519066757908</v>
+        <v>0.144065893256218</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1372,13 +1372,13 @@
         <v>85</v>
       </c>
       <c r="D35">
-        <v>0.2663943884126581</v>
+        <v>0.266394388412658</v>
       </c>
       <c r="E35">
-        <v>0.7234538650328753</v>
+        <v>0.7234538650328752</v>
       </c>
       <c r="F35">
-        <v>0.2938167438742203</v>
+        <v>0.2938167438742204</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1392,13 +1392,13 @@
         <v>86</v>
       </c>
       <c r="D36">
-        <v>0.5736866672097034</v>
+        <v>0.4530893101245041</v>
       </c>
       <c r="E36">
-        <v>0.6832336372259916</v>
+        <v>0.6093573956230762</v>
       </c>
       <c r="F36">
-        <v>0.3579032624809825</v>
+        <v>0.4278797098413298</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1412,13 +1412,13 @@
         <v>87</v>
       </c>
       <c r="D37">
-        <v>0.510919658812142</v>
+        <v>0.3920832712744233</v>
       </c>
       <c r="E37">
-        <v>0.6950903926189337</v>
+        <v>0.628720671515097</v>
       </c>
       <c r="F37">
-        <v>0.348477142679144</v>
+        <v>0.4115790210535193</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1432,13 +1432,13 @@
         <v>88</v>
       </c>
       <c r="D38">
-        <v>0.7261879056269998</v>
+        <v>0.6899563758316446</v>
       </c>
       <c r="E38">
-        <v>0.8704991910700139</v>
+        <v>0.8483425569755983</v>
       </c>
       <c r="F38">
-        <v>0.1560804360862321</v>
+        <v>0.1749101136239687</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1452,13 +1452,13 @@
         <v>89</v>
       </c>
       <c r="D39">
-        <v>0.5026016297059157</v>
+        <v>0.4166663804362242</v>
       </c>
       <c r="E39">
-        <v>0.7499944393694565</v>
+        <v>0.6928387995506464</v>
       </c>
       <c r="F39">
-        <v>0.2934898858902015</v>
+        <v>0.3453114187595375</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1472,13 +1472,13 @@
         <v>90</v>
       </c>
       <c r="D40">
-        <v>0.7704315238855011</v>
+        <v>0.7503764233194545</v>
       </c>
       <c r="E40">
-        <v>0.9609917293539744</v>
+        <v>0.9614811330946759</v>
       </c>
       <c r="F40">
-        <v>0.03900827064602567</v>
+        <v>0.0385188669053242</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1492,13 +1492,13 @@
         <v>91</v>
       </c>
       <c r="D41">
-        <v>0.7592045377273819</v>
+        <v>0.7404550478014275</v>
       </c>
       <c r="E41">
-        <v>0.9597658432776479</v>
+        <v>0.9602675573651627</v>
       </c>
       <c r="F41">
-        <v>0.04258960917205742</v>
+        <v>0.04205949565625011</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1512,13 +1512,13 @@
         <v>92</v>
       </c>
       <c r="D42">
-        <v>0.7687993925909078</v>
+        <v>0.7470939785260781</v>
       </c>
       <c r="E42">
-        <v>0.9619495525193467</v>
+        <v>0.9554698424335188</v>
       </c>
       <c r="F42">
-        <v>0.04684374352210457</v>
+        <v>0.05234118452371551</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1532,13 +1532,13 @@
         <v>93</v>
       </c>
       <c r="D43">
-        <v>0.7496974925282036</v>
+        <v>0.7321698097688492</v>
       </c>
       <c r="E43">
-        <v>0.9971475576170357</v>
+        <v>0.9971839665237002</v>
       </c>
       <c r="F43">
-        <v>0.002852442382964315</v>
+        <v>0.002816033476299789</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1552,7 +1552,7 @@
         <v>94</v>
       </c>
       <c r="D44">
-        <v>0.3894949150663778</v>
+        <v>0.3894949150663777</v>
       </c>
       <c r="E44">
         <v>0.8785987358573681</v>
@@ -1572,10 +1572,10 @@
         <v>95</v>
       </c>
       <c r="D45">
-        <v>0.3691789964565899</v>
+        <v>0.3691789964565897</v>
       </c>
       <c r="E45">
-        <v>0.8778824806841223</v>
+        <v>0.8778824806841222</v>
       </c>
       <c r="F45">
         <v>0.1288419633520589</v>
@@ -1592,13 +1592,13 @@
         <v>96</v>
       </c>
       <c r="D46">
-        <v>0.4021515474102872</v>
+        <v>0.3878507277490345</v>
       </c>
       <c r="E46">
-        <v>0.8848925390041853</v>
+        <v>0.8643685873823383</v>
       </c>
       <c r="F46">
-        <v>0.1387469995163098</v>
+        <v>0.1565802380758488</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1612,13 +1612,13 @@
         <v>97</v>
       </c>
       <c r="D47">
-        <v>0.602848985157639</v>
+        <v>0.5956039862884859</v>
       </c>
       <c r="E47">
-        <v>0.9901288170802766</v>
+        <v>0.9902242380567424</v>
       </c>
       <c r="F47">
-        <v>0.009871182919723545</v>
+        <v>0.009775761943257579</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1632,13 +1632,13 @@
         <v>98</v>
       </c>
       <c r="D48">
-        <v>0.5888678809766598</v>
+        <v>0.5699763760797616</v>
       </c>
       <c r="E48">
-        <v>0.8722600994697703</v>
+        <v>0.8548791716110304</v>
       </c>
       <c r="F48">
-        <v>0.1500817759689937</v>
+        <v>0.1652951900634266</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1652,13 +1652,13 @@
         <v>99</v>
       </c>
       <c r="D49">
-        <v>0.7077832682070367</v>
+        <v>0.6926403650370847</v>
       </c>
       <c r="E49">
-        <v>0.9169937168707779</v>
+        <v>0.9150088116147705</v>
       </c>
       <c r="F49">
-        <v>0.09036117291120201</v>
+        <v>0.0921833286296143</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1672,13 +1672,13 @@
         <v>100</v>
       </c>
       <c r="D50">
-        <v>0.6081510593875338</v>
+        <v>0.5860524714493888</v>
       </c>
       <c r="E50">
-        <v>0.8330847741029312</v>
+        <v>0.8191065114949702</v>
       </c>
       <c r="F50">
-        <v>0.1878979477557133</v>
+        <v>0.200665423617032</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1692,13 +1692,13 @@
         <v>101</v>
       </c>
       <c r="D51">
-        <v>0.7282062055827879</v>
+        <v>0.7069724604640318</v>
       </c>
       <c r="E51">
-        <v>0.9197769122870327</v>
+        <v>0.9092479535890007</v>
       </c>
       <c r="F51">
-        <v>0.09513030672816852</v>
+        <v>0.1042389039145356</v>
       </c>
     </row>
   </sheetData>
@@ -1882,13 +1882,13 @@
         <v>60</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1982,13 +1982,13 @@
         <v>65</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2142,13 +2142,13 @@
         <v>72</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2442,13 +2442,13 @@
         <v>87</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
       <c r="F37">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:6">

</xml_diff>

<commit_message>
Fixed T9, ran analysis, new graphs
</commit_message>
<xml_diff>
--- a/dmsan/bwaise/results/MCDA_baseline.xlsx
+++ b/dmsan/bwaise/results/MCDA_baseline.xlsx
@@ -479,10 +479,10 @@
         <v>0.5250328446843893</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5084190867812446</v>
+        <v>0.2227685477536643</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4915809132187554</v>
+        <v>0.7772314522463357</v>
       </c>
     </row>
     <row r="3">
@@ -599,10 +599,10 @@
         <v>0.6499145417213249</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8778272545851326</v>
+        <v>0.8643220542436826</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1323819684936061</v>
+        <v>0.1446208252063952</v>
       </c>
     </row>
     <row r="8">
@@ -623,10 +623,10 @@
         <v>0.3091609587548275</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6116771557439096</v>
+        <v>0.5434327177894198</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4047447842098413</v>
+        <v>0.4733938948918839</v>
       </c>
     </row>
     <row r="9">
@@ -647,10 +647,10 @@
         <v>0.3620185166548159</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6154564462793018</v>
+        <v>0.5738460381881468</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4122532093345651</v>
+        <v>0.4509750594913713</v>
       </c>
     </row>
     <row r="10">
@@ -671,10 +671,10 @@
         <v>0.6921888206727864</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8737372697874098</v>
+        <v>0.8598086312293285</v>
       </c>
       <c r="F10" t="n">
-        <v>0.136786239334902</v>
+        <v>0.1494026779803342</v>
       </c>
     </row>
     <row r="11">
@@ -695,10 +695,10 @@
         <v>0.4721356533617872</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5857689352793057</v>
+        <v>0.5188625936341134</v>
       </c>
       <c r="F11" t="n">
-        <v>0.441314105938786</v>
+        <v>0.5023898737537218</v>
       </c>
     </row>
     <row r="12">
@@ -719,10 +719,10 @@
         <v>0.7447688187902374</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9259958224920952</v>
+        <v>0.9002138881024789</v>
       </c>
       <c r="F12" t="n">
-        <v>0.07400417750790486</v>
+        <v>0.09978611189752094</v>
       </c>
     </row>
     <row r="13">
@@ -743,10 +743,10 @@
         <v>0.4046322827814371</v>
       </c>
       <c r="E13" t="n">
-        <v>0.789637417678884</v>
+        <v>0.7244050160684078</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2103625823211161</v>
+        <v>0.2755949839315923</v>
       </c>
     </row>
     <row r="14">
@@ -767,10 +767,10 @@
         <v>0.3620185166548159</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6154564462793018</v>
+        <v>0.5738460381881468</v>
       </c>
       <c r="F14" t="n">
-        <v>0.4122532093345651</v>
+        <v>0.4509750594913713</v>
       </c>
     </row>
     <row r="15">
@@ -791,10 +791,10 @@
         <v>0.6921888206727864</v>
       </c>
       <c r="E15" t="n">
-        <v>0.8737372697874098</v>
+        <v>0.8598086312293285</v>
       </c>
       <c r="F15" t="n">
-        <v>0.136786239334902</v>
+        <v>0.1494026779803342</v>
       </c>
     </row>
     <row r="16">
@@ -815,10 +815,10 @@
         <v>0.6729456182270112</v>
       </c>
       <c r="E16" t="n">
-        <v>0.8954214936130447</v>
+        <v>0.8788407057929699</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1147919572510599</v>
+        <v>0.1296768366373445</v>
       </c>
     </row>
     <row r="17">
@@ -839,10 +839,10 @@
         <v>0.4126776354512215</v>
       </c>
       <c r="E17" t="n">
-        <v>0.7329567446632728</v>
+        <v>0.6942695365180909</v>
       </c>
       <c r="F17" t="n">
-        <v>0.2883098614051222</v>
+        <v>0.3227899650669473</v>
       </c>
     </row>
     <row r="18">
@@ -1103,10 +1103,10 @@
         <v>0.4197763838391815</v>
       </c>
       <c r="E28" t="n">
-        <v>0.561993791380736</v>
+        <v>0.4233067709684146</v>
       </c>
       <c r="F28" t="n">
-        <v>0.4468019021318038</v>
+        <v>0.5884870768418804</v>
       </c>
     </row>
     <row r="29">
@@ -1127,10 +1127,10 @@
         <v>0.4992126290541916</v>
       </c>
       <c r="E29" t="n">
-        <v>0.5487710217178979</v>
+        <v>0.4079095200044974</v>
       </c>
       <c r="F29" t="n">
-        <v>0.4642226902831631</v>
+        <v>0.6008026351603301</v>
       </c>
     </row>
     <row r="30">
@@ -1151,10 +1151,10 @@
         <v>0.7254007048602344</v>
       </c>
       <c r="E30" t="n">
-        <v>0.8633910668752239</v>
+        <v>0.8187598662855726</v>
       </c>
       <c r="F30" t="n">
-        <v>0.136608933124776</v>
+        <v>0.1812401337144274</v>
       </c>
     </row>
     <row r="31">
@@ -1175,10 +1175,10 @@
         <v>0.441158559173889</v>
       </c>
       <c r="E31" t="n">
-        <v>0.6755971720939401</v>
+        <v>0.5724224368103152</v>
       </c>
       <c r="F31" t="n">
-        <v>0.32440282790606</v>
+        <v>0.4275775631896847</v>
       </c>
     </row>
     <row r="32">
@@ -1199,10 +1199,10 @@
         <v>0.2052027779755892</v>
       </c>
       <c r="E32" t="n">
-        <v>0.6443363925673763</v>
+        <v>0.6195447123585156</v>
       </c>
       <c r="F32" t="n">
-        <v>0.3772071169015823</v>
+        <v>0.4015400151485282</v>
       </c>
     </row>
     <row r="33">
@@ -1295,10 +1295,10 @@
         <v>0.4530893101245041</v>
       </c>
       <c r="E36" t="n">
-        <v>0.6093573956230762</v>
+        <v>0.5862029576185354</v>
       </c>
       <c r="F36" t="n">
-        <v>0.4278797098413298</v>
+        <v>0.4477419125491551</v>
       </c>
     </row>
     <row r="37">
@@ -1391,10 +1391,10 @@
         <v>0.7503764233194545</v>
       </c>
       <c r="E40" t="n">
-        <v>0.9614811330946759</v>
+        <v>0.9474680615893214</v>
       </c>
       <c r="F40" t="n">
-        <v>0.0385188669053242</v>
+        <v>0.05253193841067868</v>
       </c>
     </row>
     <row r="41">
@@ -1487,10 +1487,10 @@
         <v>0.3894949150663777</v>
       </c>
       <c r="E44" t="n">
-        <v>0.8785987358573681</v>
+        <v>0.8390467454170564</v>
       </c>
       <c r="F44" t="n">
-        <v>0.1214012641426319</v>
+        <v>0.1609532545829435</v>
       </c>
     </row>
     <row r="45">
@@ -1722,13 +1722,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1938,13 +1938,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -2349,10 +2349,10 @@
         <v>3</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -2373,10 +2373,10 @@
         <v>2</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">

</xml_diff>